<commit_message>
Modificado cadastro de indice
</commit_message>
<xml_diff>
--- a/web/uploads/documentosTeste.xlsx
+++ b/web/uploads/documentosTeste.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Nome</t>
   </si>
@@ -372,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A9"/>
+      <selection activeCell="A5" sqref="A5:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,61 +428,6 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>265916</v>
-      </c>
-      <c r="C5">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>96377</v>
-      </c>
-      <c r="C6">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>186664</v>
-      </c>
-      <c r="C7">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>12253</v>
-      </c>
-      <c r="C8">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>39</v>
-      </c>
-      <c r="C9">
-        <v>2016</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Conserto da função para fazer upload de documentos.
Falta: mensagem avisando que não houve upload de algumas informações pois estavam null
</commit_message>
<xml_diff>
--- a/web/uploads/documentosTeste.xlsx
+++ b/web/uploads/documentosTeste.xlsx
@@ -375,7 +375,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,9 +399,6 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>91381</v>
-      </c>
       <c r="C2">
         <v>2016</v>
       </c>

</xml_diff>

<commit_message>
Alteração no indice da tabela de upload
</commit_message>
<xml_diff>
--- a/web/uploads/documentosTeste.xlsx
+++ b/web/uploads/documentosTeste.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -81,6 +81,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -88,7 +91,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -126,9 +129,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -163,7 +166,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -198,7 +201,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -375,7 +378,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,6 +402,9 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2">
+        <v>999</v>
+      </c>
       <c r="C2">
         <v>2016</v>
       </c>

</xml_diff>